<commit_message>
Fixed strlen operation priority
</commit_message>
<xml_diff>
--- a/design/precedence_table.xlsx
+++ b/design/precedence_table.xlsx
@@ -137,7 +137,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,8 +172,14 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Cascadia Code"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -210,8 +216,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -439,11 +451,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -468,6 +497,69 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -485,66 +577,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -579,6 +611,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -877,7 +914,7 @@
   <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -888,127 +925,129 @@
   <sheetData>
     <row r="1" spans="1:23" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1"/>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="34" t="s">
+      <c r="F1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="34" t="s">
+      <c r="I1" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="34" t="s">
+      <c r="K1" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="34" t="s">
+      <c r="N1" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="34" t="s">
+      <c r="O1" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="P1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="36" t="s">
+      <c r="Q1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="37" t="s">
+      <c r="R1" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="34"/>
     </row>
     <row r="2" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="M2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="N2" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="O2" s="29" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="30"/>
-      <c r="Q2" s="31" t="s">
-        <v>7</v>
-      </c>
-      <c r="R2" s="32" t="s">
-        <v>9</v>
-      </c>
-      <c r="S2" s="14" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="S2" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="36"/>
+      <c r="V2" s="36"/>
     </row>
     <row r="3" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="5" t="s">
@@ -1059,19 +1098,19 @@
       <c r="R3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="16" t="s">
+      <c r="S3" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="T3" s="17"/>
-      <c r="U3" s="17"/>
-      <c r="V3" s="17"/>
-      <c r="W3" s="17"/>
+      <c r="T3" s="38"/>
+      <c r="U3" s="38"/>
+      <c r="V3" s="38"/>
+      <c r="W3" s="38"/>
     </row>
     <row r="4" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -1130,10 +1169,10 @@
       </c>
     </row>
     <row r="5" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -1192,10 +1231,10 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1251,10 +1290,10 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1310,10 +1349,10 @@
       </c>
     </row>
     <row r="8" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1369,10 +1408,10 @@
       </c>
     </row>
     <row r="9" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1393,14 +1432,14 @@
       <c r="H9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="38" t="s">
+      <c r="I9" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="40"/>
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="40"/>
+      <c r="N9" s="41"/>
       <c r="O9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1418,10 +1457,10 @@
       </c>
     </row>
     <row r="10" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1442,12 +1481,12 @@
       <c r="H10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="41"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="42"/>
-      <c r="N10" s="43"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="44"/>
       <c r="O10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1465,10 +1504,10 @@
       </c>
     </row>
     <row r="11" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="19" t="s">
+      <c r="A11" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1489,12 +1528,12 @@
       <c r="H11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I11" s="41"/>
-      <c r="J11" s="42"/>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="42"/>
-      <c r="N11" s="43"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="44"/>
       <c r="O11" s="4" t="s">
         <v>7</v>
       </c>
@@ -1512,10 +1551,10 @@
       </c>
     </row>
     <row r="12" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1536,12 +1575,12 @@
       <c r="H12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I12" s="41"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
-      <c r="M12" s="42"/>
-      <c r="N12" s="43"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="44"/>
       <c r="O12" s="4" t="s">
         <v>7</v>
       </c>
@@ -1559,10 +1598,10 @@
       </c>
     </row>
     <row r="13" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1583,12 +1622,12 @@
       <c r="H13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I13" s="41"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
-      <c r="M13" s="42"/>
-      <c r="N13" s="43"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="44"/>
       <c r="O13" s="4" t="s">
         <v>7</v>
       </c>
@@ -1606,10 +1645,10 @@
       </c>
     </row>
     <row r="14" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="13" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1630,12 +1669,12 @@
       <c r="H14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="44"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="45"/>
-      <c r="M14" s="45"/>
-      <c r="N14" s="46"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
+      <c r="N14" s="47"/>
       <c r="O14" s="4" t="s">
         <v>7</v>
       </c>
@@ -1653,10 +1692,10 @@
       </c>
     </row>
     <row r="15" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="14" t="s">
         <v>7</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1710,12 +1749,10 @@
       </c>
     </row>
     <row r="16" spans="1:23" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="20" t="s">
-        <v>9</v>
-      </c>
+      <c r="B16" s="31"/>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
@@ -1765,10 +1802,10 @@
       </c>
     </row>
     <row r="17" spans="1:20" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="18"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="6" t="s">
         <v>9</v>
       </c>
@@ -1818,10 +1855,10 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="15" t="s">
         <v>7</v>
       </c>
       <c r="C18" s="10" t="s">

</xml_diff>